<commit_message>
Test <Listener and Screenshot capturing
</commit_message>
<xml_diff>
--- a/src/test/java/resources/excel/TestData.xlsx
+++ b/src/test/java/resources/excel/TestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\neeth\Documents\GitHub\Repo\DataDrivenFramwork\src\test\java\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16C2FB1E-A5F6-49CE-8FFB-204572A1779D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E760A39-B229-4B39-8B28-85B1E2700624}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -409,7 +409,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2:D4"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>